<commit_message>
organize client and server code in folders.
add some more logic
</commit_message>
<xml_diff>
--- a/docs/libro ventas prueba.xlsx
+++ b/docs/libro ventas prueba.xlsx
@@ -292,22 +292,22 @@
   </sheetPr>
   <dimension ref="A1:P65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="12" min="6" style="2" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="2" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="4" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="5" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="4" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="4" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="4" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="4" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="5" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1023" min="18" style="2" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.89068825910931"/>

</xml_diff>